<commit_message>
Add business_layer final version
</commit_message>
<xml_diff>
--- a/business_layer/Documents/cv_infos.xlsx
+++ b/business_layer/Documents/cv_infos.xlsx
@@ -462,6 +462,11 @@
           <t>Competence</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -537,28 +542,17 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>Stagiaire Développeur chez GSDEV, Derb-Omar, Casablanca,
-Maroc.,Développement d'une plateforme d'apprentissage en ligne en
-utilisant PHP, Bootstrap, HTML, CSS, et JavaScript.,</t>
+Maroc.,</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Cycle d’ingénieur : 2ème année cycle d’ingénieur dans l’Intelligence Artificielle
-et Génie Informatique à l'ENSAM de Casablanca.,Cycle d’ingénieur : 1ère année cycle d’ingénieur dans l’Intelligence Artificielle
-et Génie Informatique à l'ENSAM de Casablanca.,Diplôme d'études universitaires générales :
-     DEUG , Sciences Mathématiques et Informatique (SMI) à la Faculté
-des sciences Ain Chock.,Diplôme de Baccalauréat en Science physiques,</t>
+          <t>Cycle d’ingénieur :,Cycle d’ingénieur :,Diplôme d'études universitaires générales :,Diplôme de Baccalauréat en Science physiques,</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Java,Python,R,C,C#,PHP,Javascript,Angular,React,Spring Boot,Hibernate,Bootstrap,NumPy,Pandas,Matplotlib,Seaborn,Scikit-Learn,MySQL,Oracle,MongoDB,développer des applications mobiles avec Java,connaissance de la plateforme Unity et de son fonctionnement 
-pour le développement d'applications AR et de jeux.,Développement d'un site e-commerce complet pour la
-vente de survêtements et de vestes en utilisant Spring Boot,
-Spring Data, Angular, et Spring Data REST.,Analyse des données sur le problème des stages pour les
-étudiants de l'ENSAM en utilisant le langage R.,Développement d'un site web pour la  location de voiture
-(Interface avec html&amp;css et back-end avec PHP,SQL),Réalisation d'un logiciel de gestion des études (Python OOP,
-Tkinter, SqlLite).,HCIA-5G Huawei Certification,Teamwork Skills,Design Thinking for Innovation,CLA: Programming Essentials in C,NDG Linux Unhatched,Engagement,Ponctualité,Adaptabilité,Esprit d'équipe,Volonté d’apprendre,Capacité d’écoute,</t>
+          <t>Java,Python,R,C,C#,PHP,Javascript,Angular,React,Spring Boot,Hibernate,Bootstrap,NumPy,Pandas,Matplotlib,Seaborn,Scikit-Learn,MySQL,Oracle,MongoDB,Unity,</t>
         </is>
       </c>
       <c r="I3" t="n">

</xml_diff>